<commit_message>
all done except explanation
</commit_message>
<xml_diff>
--- a/balance.xlsx
+++ b/balance.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mykad\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mykad\Desktop\balance_calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C674D3B-FA9A-4449-A88E-D1D181A5F86B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60701E4C-6685-47F2-A0FA-C7CD8B320260}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,10 +30,10 @@
     <t>mass_g</t>
   </si>
   <si>
-    <t>voltage_v</t>
+    <t>attempt</t>
   </si>
   <si>
-    <t>attempt</t>
+    <t>voltage_mv</t>
   </si>
 </sst>
 </file>
@@ -354,20 +354,20 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>